<commit_message>
Updated the folder structure
</commit_message>
<xml_diff>
--- a/data/News.xlsx
+++ b/data/News.xlsx
@@ -1074,10 +1074,10 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="15.1047619047619" defaultRowHeight="15" customHeight="1"/>
@@ -2112,7 +2112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2758,607 +2758,6 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Predictions for end to NJ's county line: More accountability, maybe more money in politics</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2024-04-03</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Nancy Solomon</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Abolishing New Jersey’s “county line” ballot system could radically reshape the state’s politics, from increasing the number of competitive primaries to holding legislators accountable for unpopular votes in Trenton.
-The county line has been a potent tool for the state’s political machines by helping them sway races and pick the likely winners months before voters go to the ballots. The ballot system groups candidates endorsed by county political party organizations into a single row or column on primary ballots, signaling to voters a stamp of approval from their party.
-But on Friday, a federal judge ordered a temporary injunction against the Democratic Party’s use of the county line in June’s primary. The lawsuit was brought by U.S. Senate candidate and current Rep. Andy Kim, whose attorneys say the judge’s ruling suggests a separate lawsuit that aims to permanently end the system would likely prevail as well. And even if the judge doesn’t eliminate the county line, the Legislature might. Leaders from both major parties have said they’re open to change, so long as it isn’t imposed by the courts.
-If the county line system is eliminated permanently, longtime political observers said New Jersey's primary races will be more competitive and will force legislators to be more responsive to their constituents rather than the party chairs who run the political organizations. Some political scientists and elected officials predict that without the party bosses serving as gatekeepers, New Jersey could see more money in primaries, or political extremists could vie for attention during polarizing campaigns.
-Despite a record number of open seats in the state Legislature in 2023, only 13% of state Senate and Assembly seats had contested primaries. The national average in 2022 was 24%, according to Ballotpedia, a nonprofit and nonpartisan election information hub.
-Micah Rasmussen, director of the Rebovich Institute for New Jersey Politics, said that’s because other potential primary candidates are dissuaded from running when political organizations award the county line.
-Eliminating the line “could be the great equalizer,” he said, because county party chairs will hold less power. Candidates will instead need to appeal to many different constituencies and groups to build support, according to Rasmussen and other observers.
-“I think we're going to see more interesting things come before the Legislature,” said Hetty Rosenstein, the former director of the state’s Communication Workers of America.” I think having to have your own base of support and having to make sure that you are responsive to your district will cause more legislators to function independently and make an attempt to make a name for themselves.”
-Researchers say many voters tend to tick off every name on the line, giving the endorsed candidates a huge advantage.
-If they can’t rely on that advantage conferred by the party chairs, Rasmussen and others say, state legislators will become more wary of rushing through legislation that’s popular with the political establishment, but controversial among constituents — like a proposed bill to gut the state’s public records act, or last year’s bill that weakened campaign finance and pay-to-play laws despite a stated purpose of increasing election transparency.
-Although New Jersey's most powerful Democratic legislative leaders supported those measures, good governments decried them and said they would open the state up to more corruption and less public scrutiny.
-“The sense that we can do what we want, it's not going to matter, we have these tools that shield us from public accountability — I hope that goes away, Rasmussen said.
-But the county party chairs will still matter, Rasmussen said, because they can still raise money and have organizations that can mobilize voters.
-Republican state Sen. Jon Bramnick, who is running for governor in 2025, also sees a huge shift coming, but he is not certain it will be positive.
-He said the county line works well if the process is democratic. In some counties, party chairs award their organizations’ endorsements themselves. But in others, the organizations hold conventions and award their endorsements via secret votes among delegates.
-“I like that because there's a filtering process that sometimes rejects the most extreme person and sometimes rejects the wealthiest person because these are true representatives of each district in the county,” Bramnick said.
-But the county line system never fully removed money from the political equation. Jon Corzine and Phil Murphy both made large donations to county Democratic organizations before securing endorsements for their successful runs for governor.
-If the county line is abolished before next year’s gubernatorial election, it could significantly change the dynamics of the race, especially among the large Democratic field expected to run. None of the anticipated candidates has a statewide base; instead, each one would have to build that support from the ground up rather than rely on deals with county bosses.
-“I think we're going to see a big shakeup because up until this point, the candidates who have gotten into the race are all very strong within their own regions,” Rasmussen said. “It's a recalculation. It's a recalibration. It's a different kind of campaign that's not aimed at insiders so much, but it's aimed at those who vote in primaries.”
-Some members of the county party organizations have been advocating for a more democratic process. Rebecca Scheer, a member of the Essex County Democratic Committee, wants to see the county line abolished, but wants the party to remain strong.
-“Some people are looking at it that this is just going to be all sunshine and rainbows,” Scheer said. “But there's just a culture of machine politics in New Jersey and that's not going away just because the line went away.”
-Scheer and other progressive members of the committee have been calling for a convention in Essex, one of several large Democratic committees where the party chair endorses candidates on behalf of the organization himself. She believes that reform could happen now that the county line's power is in jeopardy.
-“I think having a strong Democratic Party is good, big-D Democratic. I see a lot of problems with the Democratic Party and things I'd like to change, but it's still my party,” Scheer said. “And I think it's great that we can have this apparatus to turn out the vote. I just think we need to be more small-d democratic about it.”
-</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>25</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/344260/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Texas Gov. Abbott helped spur NY’s ‘migrant crisis.’ He’s in town on Thursday.</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2024-04-03</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Arya Sundaram</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Texas Gov. Greg Abbott's politics have shaped New York City's current immigration debate from more than 1,700 miles away.
-Abbott will return to Manhattan to headline the annual New York state Republican Committee gala and fundraiser on Thursday. Political analysts said his appearance at one of the GOP's leading fundraisers highlights a key campaign strategy for the party in 2024: leaning into voters' discontent over immigration and playing up fissures among Democrats on the issue.
-New York has become emblematic of that strain and division two years into a migrant crisis that has reached far beyond Texas due to Abbott's efforts. State Republican Committee Chair Ed Cox said campaigning on immigration is how he plans to help the GOP retain control of the U.S. House in November. The GOP flipped four Democratic House seats in New York in 2022, more than any other state.
-Two years ago, Abbott began busing migrants from Texas to New York City and other Democratic-led cities in a brazen rebuke of the Biden administration’s border controls. Adams and other Democrats labeled the busing policy an inhumane “political stunt,” but the tactic succeeded in dividing Democrats and making immigration a local issue in states far from the southern border.
-Abbott’s office did not respond to multiple requests for comment ahead of his visit to the Hilton Hotel in Midtown on Thursday evening.
-“The big issue that's really surpassed the economy is … illegal aliens caught crossing our border,” Cox said. “Who better to represent that issue than Gov. Abbott, the governor of Texas, where the caravans aim?”
-Democratic Party leaders say the Republicans’ campaign rhetoric on immigration will fail, and point to Democrat Tom Suozzi's recent triumph in flipping Republican George Santos' Long Island congressional seat. In the special election, the GOP tried to portray Suozzi as being weak on border security and immigration. Democrats highlighted Republicans’ unwillingness to act on immigration reform, including compromises forged by a bipartisan group of Senate lawmakers.
-“Instead of inviting Gov. Abbott to speak at a gala, we encourage members of the NY GOP to urge their far-right Republican colleagues in Congress to pass comprehensive immigration reform, something they have blocked for decades,” City Hall spokesperson Kayla Mamelak said in a statement.
-New York City's migrant crisis seemed to spring out of nowhere in 2022. Busloads of migrants from Texas began showing up at the Port Authority Bus Terminal, unannounced and at all hours.
-All told, since the spring of 2022, Abbott has spent more than $148 million to bus over 100,000 migrants to predominantly Democratic-run cities, according to a tally reported on Feb. 21 by the Texas Tribune.
-New York City, Chicago, Denver, Washington, D.C., Los Angeles and Philadelphia are among the leading destinations. Abbott has said the tactic aimed to “bring the border” to northern cities and states.
-The governor has also sought to greatly expand Texas’ powers to secure the southern border and enforce immigration laws. The Supreme Court in March gave Texas permission to arrest and prosecute migrants suspected of crossing the border without legal authorization, before a federal appeals court blocked Texas from enforcing the state measure.
-Adams has condemned Abbott's busing initiative as "morally bankrupt" and "devoid of concern" for the well-being of migrants, whom he claims are being used as “political pawns.” Adams has also claimed that "Abbott is using this crisis to hurt Black-run cities," noting that many of the cities that have become top migrant destinations have Black mayors.
-But the mayor has also criticized the Biden administration’s handling of the crisis and complained of a lack of federal coordination and financial support — sounding some of the same alarms as the Democratic president’s Republican critics and, increasingly, other Democratic leaders.
-New York City has set up over 200 shelters for the new arrivals. The Adams administration estimates the cost of housing and caring for the migrants through June 2025 will reach $10.5 billion.
-Abbott’s buses aren’t the only way migrants are landing in New York, as many migrants buy their own bus and plane tickets to the city. But in an age in which social media is often the loudest messenger, immigration researchers said Abbott’s efforts have spread awareness of New York City’s unique right-to-shelter policies, which guarantee every new arrival a shelter bed, at least temporarily.
-As of late March, Abbott’s office claims Texas has sent some 40,300 migrants to New York City since 2022. That’s just a fraction of the more than 180,000 migrants who have funneled through the city’s shelter system since spring 2022. Roughly 65,000 are currently staying in city shelters.
-“He certainly has forced other parts of the country to deal with the influx of people across the border in a way that they might not otherwise,” said Tyler Anbinder, an immigration historian and professor at George Washington University.
-Siena College pollster Steven Greenberg said his organization hadn’t even surveyed New York voters on immigration until a few years ago. He said immigration “has not been an issue of that kind of significance in New York, certainly not in this century.” It’s now showing up as a No. 1 issue in both statewide and New York City surveys.
-Basil Smikle, a Columbia University lecturer and former executive director of the state Democratic Party, said Abbott’s actions have also sown division among more established immigrants and Black voters, as the Adams administration has blamed the migrant crisis for a litany of budget worries and spending cuts.
-“There's a feeling, particularly among communities of color….who have this sense that there's not enough to go around,” Smikle said. “And the more you bring in, the more that come in, the less there is for the rest of us.”
-Cox, the state GOP chair, said he believes focusing on immigration will be a winning strategy for Republicans. That’s notwithstanding the party’s loss in New York’s 3rd Congressional District race, where Republican Mazi Pilip assailed Suozzi’s record on immigration in looping campaign ads.
-Cox claimed several factors gave Suozzi the upper hand in the election, including his name recognition, reputation as a moderate, prior incumbency in the seat before Santos, and heavy Democratic spending.
-All those factors combined so Suozzi could “deaden” the issue of immigration, Cox said. “But it is not going to work nationally,” he claimed.
-Jim McLaughlin, a Republican strategist whose consulting firm has advised former President Donald Trump and gubernatorial candidate Lee Zeldin in his closer-than-expected race against Gov. Kathy Hochul in 2022, agreed with Cox.
-“People get it right now: That every state is a border state,” McLaughlin said.
-He added: “Immigration has become the symbol for the failure of the Democrats and Joe Biden.”
-McLaughlin said voters see immigration as something that exacerbates bedrock issues like crime, education and the economy.
-“The ads,” McLaughlin said, “ literally write themselves against the Democrats on the border issue.”
-Jefrey Pollock, a Democratic consultant and pollster who is the president of the New York-based Global Strategy Group, said he predicts other Democrats vying in contentious races across the state will “take a page” from Suozzi’s successful playbook.
-When Suozzi was accused of helping to create New York's migrant crisis, he leaned into the issue of immigration in his stump speeches and messaging. He sometimes distanced himself from Biden and his party, and campaigned on tougher border control measures. He also attacked Senate Republicans for abandoning a bipartisan border deal earlier this year that included stronger immigration enforcement policies long sought by conservatives.
-“The big lesson from that race was to push back on the Republicans,” Pollock said.
-“It can't be just defense; it has to be offense,” he added.
-Jay Jacobs, the chair of the New York State Democratic Party, said that’s how the party will move forward this election year.
-“We're not gonna avoid the argument. We're gonna lean into it,” Jacobs said of immigration. “And we're going to be crystal clear about what the Republicans have failed to do and why they have failed to do it.”
-But Fordham University political science professor Christina Greer said Democrats remain vulnerable, given their inability to address voters’ concerns about scarce resources, as New York City grapples with a housing crisis and budget cuts.
-“You can't say that we've got limited resources, and we keep finding billions upon billions of dollars for international affairs. So either we have the money or we don't,” Greer said. “I think that's where it's getting a little more tense this particular election year.”
-Smikle also voiced concerns about what he sees as a harsher tone on immigration among New York Democrats, who have typically taken a more welcoming stance toward immigrants.
-“The challenge for the Democrats is not to fall into the Republicans' game plan,” Smikle said. “Because they don't win by adopting their language. They win by offering better policy alternatives.”
-While Smikle said some Democrats’ rhetoric around immigration has been “concerning,” he added, “There is an audience for that, even (in) a Democratic city like New York.”
-</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>27</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/344261/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>NJ’s Kim vs. Murphy Senate race is wild. Here are 5 reasons why.</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2024-03-22</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Nancy Solomon</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A federal judge could rule any day on the unique New Jersey ballot system that gives candidates who are endorsed by political parties a huge advantage.
-The debate over New Jersey’s arcane “county line” ballot design has been thrust into the spotlight in an election season full of wild and woolly Democratic Party county conventions, where U.S. Senate race frontrunners Rep. Andy Kim and first lady Tammy Murphy have battled for the political organizations’ endorsements.
-Kim has won many of those endorsements, but in a majority of New Jersey’s most Democratic counties, they’re awarded directly by party leaders who back Murphy, so she’ll get preferential treatment on most primary ballots. Kim is suing to end the county line ballot system ahead of the primary. If he wins, he’d upend a system party bosses have long used to sway elections in a state where their political machines reign supreme.
-Kim and the progressive activists supporting him said the ground has shifted on the issue.
-“You can see from the number of people who showed up [in court], the number of candidates and elected officials all over New Jersey right now that are speaking out against this, there are a lot of people that have deep concerns about this,” Kim said. “I think there are a lot of people that haven't spoken out before that now are.”
-It’s the first time New Jersey has seen a competitive Democratic primary for Senate in decades, and the first time the unusual ballot layout has become a statewide campaign issue. Here are five remarkable developments that got us here.
-Not all county committees award their endorsements through votes at conventions; in some cases, party bosses decide on those endorsements themselves. When committees do hold conventions, they usually invite the candidates to speak to their memberships, which comprise hundreds of delegates who often hold elected and appointed positions in local government themselves.
-A candidate who wins the committee endorsement also gets the preferential ballot placement known as the county line in 19 of New Jersey’s 21 counties. The county line groups party-endorsed candidates on the ballot in a slate with other well-known Democrats — in this case, with the sitting U.S. president at the head of the list.
-“Many, if not most counties do it the same way. We've got 1,000 people in there. You've got to sing for your supper, one candidate after the other,” Gov. Phil Murphy said during the December episode of WNYC’s “Ask Governor Murphy” call-in show. “Just because the chair says ‘I like candidate A,’ you have to go through a very serious process with 1,000 people in the room.”
-But Senate candidate Patricia Campos-Medina said she wasn't allowed inside the building at last Saturday's Camden County Democratic Committee convention.
-Tammy Murphy said in her stump speech that the Senate needs more women to fight for the issues important to them. But she hasn’t commented directly about how the race's only other female candidate was shut out. Her campaign referred questions about the decision to the Camden County Democratic Committee, which hasn’t responded to a request for comment made Thursday.
-“I thought it was absolutely terrible of Tammy,” said Kate Delany, president of South Jersey Progressive Democrats. “If she is going to run as the feminist candidate, it’s disgraceful.”
-Murphy offered some limited comments to reporters at another convention in Atlantic County the same weekend
-"We're all playing by the same rules in the counties. We're all showing up and trying to do our best," she said.
-The Camden committee had only announced the convention to its members a few days before, and Kim said he decided not to attend when he couldn’t get a response from the committee about whether he would be allowed inside. That meant Murphy was the only Senate candidate to attend.
-Video of Campos-Medina arguing with a wall of large men wearing sunglasses and backward-turned baseball caps circulated on social media.
-“These men acted more like bouncers at a club than Democratic party officials helping to facilitate a Democratic party meeting,” Campos-Medina wrote in a guest column for the Star-Ledger this week, calling for an end to the county line system.
-Inside, the committee awarded the entire county line at once — including President Joe Biden, Murphy, and Rep. Donald Norcross — by acclamation. No other Senate candidates were mentioned.
-“I am proud of the overwhelming support my campaign has received in Camden, as well as from our community members, faith leaders, and elected officials,” Murphy said in a press release after the vote.
-“Thank you Cape May for a fantastic day, lot of laughs, and thoughtful conversations,” Murphy tweeted two days before the Cape May Democratic Committee met for its convention. As she did ahead of other conventions, she spent time on the ground campaigning for convention votes.
-Yet when the convention happened, the leadership of the Cape May County Democrats recommended the committee cancel its vote, and not offer an endorsement at all.
-Cape May’s Democratic committee has not yet responded to a request to explain the reason for the cancellation.
-“She also spent the weekend in Cape May, so was clearly making a play there. If she had the votes, they’d have endorsed,” tweeted Micah Rasmussen, director of the Rebovich Institute for New Jersey Politics.
-Although Cape May County is home to just 1% of the state's registered Democrats, each convention loss has added to the perception that Murphy isn’t the preferred choice of the party base.
-Since Kim entered the race the day after incumbent Sen. Bob Menendez was indicted on corruption and bribery charges, Kim has had the support of many progressive activists across the state, including members of the groups Action Together NJ, Essex Rising, South Jersey Progressive Democrats and NJ 11th for Change. They like his anticorruption message and are turned off by what many argue is the nepotism inherent in a candidacy by the governor’s wife.
-But when Murphy announced her candidacy, eight party bosses from the counties with the most powerful machines and largest number of Democratic voters endorsed her.
-That usually means “game over” for any competitor in the primary. And even though Kim won most of the conventions where delegates voted on secret ballots, Murphy will still get the preferential “county line” treatment on the primary ballots available to at least two-thirds of registered Democrats in the state, according to Gothamist’s calculation. In most of the counties with the largest numbers of Democrats, party bosses awarded Murphy the “county line” without any convention at all.
-Progressive activists, and specifically progressive women, have been organizing in New Jersey since the 2017 women’s march. And some say that experience with networking, door-knocking and get-out-the-vote efforts is helping them organize for Kim.
-“They felt empowered when they succeeded in electing three experienced public servants who had never run for elected office before – Mikie Sherrill, Tom Malinowski, and Andy Kim – to Congress,” Amy Higer, one of the founders of SOMA Action, said. Her group is made up of residents of South Orange and Maplewood, but they now work across the state.
-SOMA Action and many other groups have begun volunteering for Kim, phone banking, holding events, and attending visibility rallies outside the conventions.
-Jersey City Mayor Steven Fulop, who is running in the 2025 gubernatorial race, announced on Monday he was switching his endorsement from Murphy to Kim — saying the activists helped convince him to make the change.
-“I told [Andy Kim] it’s not always comfortable to admit a mistake but clearly I made one here and this convention season has demonstrated he is the better candidate to represent NJ,” Fulop tweeted. “The backbone of our party volunteers and activists have spoken loudly and we should listen to them.”
-Fulop told NJ Spotlight News that he became increasingly frustrated with the way Kim had been shut out from making his case at the largest county conventions and called on Murphy to drop out.
-Before this primary fight, the number of people in New Jersey who understood the “county line” was likely minuscule.
-It would require intervention by the federal judge presiding over Kim’s lawsuit, filed in February and argued in court this week, to stop the line before the June primary. But there is little doubt that the conversation about it has already changed.
-“Now, when I talk to folks, I've actually had people come up to me and say, ‘Hey, did you see this? Do you know about the line?’ This has never happened before,” said Arati Kreibich, who ran against her incumbent representative in 2020 without the county line and lost. “That in itself is a huge win compared to anything else that has happened. So I think we've already won in a real grassroots, public awareness way. And I don't think there's any letting the genie back in the bottle.”
-But Kim is suing the clerks of the 19 counties that use the line system. The progressive activists are calling for change. And the state attorney general, New Jersey's top law enforcement official, recently said he thinks the practice is unconstitutional.
-“Look I just ask for us to have a fair ballot here. I’m not asking for any advantages given to me,” Kim told the judge during a nine-hour hearing in federal court on Monday, noting that Senate seats rarely open up. Menendez has been in the Senate since 2006, when he was appointed to his first term by Gov. Jon Corzine. “It is the only time I'll be able to step up and run for Senate in this way. I want to run for the Senate and serve the country, and I want to appeal to the voters in a fair way.”
-Former candidates for Congress and the New Jersey Working Families Alliance filed a different lawsuit challenging the county line in 2021. That case is slowly winding its way through the legal process.
-But the public pressure against the county line is prompting elected officials to take a stand against it for the first time.
-The state Senate's Democratic president, the speaker of the General Assembly, and the Republican Senate and Assembly minority leaders all announced in a rare joint letter this week they would consider legislation to reform the ballot design. But they do not want to begin that work until next year.
-LeRoy Jones — who chairs the Essex County Democratic Committee, home to the state’s largest number of registered Democrats, as well as the state Democratic Committees — said he is now open to discussing reform. But again, he’s not looking to make any changes ahead of the Senate primary.
-Monmouth’s Democratic committee was the first to hold a convention, on Feb. 10, and the hourlong wait to enter the building was the first clue that something different was happening.
-Despite leadership support for Murphy, who was on her home turf — she and the governor live in Middletown —an overwhelming majority of members of the committee voted for Kim.
-That scene was repeated in all but one of the conventions where members were allowed to take secret votes. Murphy won the endorsement in the counties where the party chair called for a raise of hands, in view of party leaders
-And after members had turned in their paper ballots on Feb. 24 in Hunterdon County, Chair Arlene Quiñones Perez announced the executive committee had decided that anyone who received 30% of the vote or more would share the line of the ballot. Kim's supporters quickly understood this would weaken his position, because Kim needed the line in the smaller, more democratically run county committees to counter the big committees that were supporting Murphy, usually without a convention vote.
-Shouting and chaos ensued, and ultimately rank-and-file committee members were able to force a vote that overturned the executive committee’s decision. Kim won 62% of the endorsement vote and Tammy Murphy won 33%, which would have put the first lady on the ballot’s party line along with Kim under the committee chair's original plan.
-Elizabeth Redwine is a member of the West Orange Democratic Committee in Essex County. She and other women who have been active since the Women’s March at the beginning of the Trump presidency have been fighting for a more open democratic process in New Jersey.
-She was able to get Jones, the Essex County chair, to attend a meeting at her house to discuss making the system more democratic. Jones told Gothamist in February his county wouldn’t have an endorsement vote among its members and that he was awarding Murphy the county line based on conversations he’d had with other local leaders. Redwine is happy Jones now seems open to reform.
-“I am glad to see his openness to a fairer ballot,” Redwine said, but she wants to see the timeline moved up. “The issue is that New Jersey needs fair ballots for the June primary.”
-</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>23</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/344096/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>NY’s Shirley Chisholm, still ‘Unbought and Unbossed,’ debuts on Netflix</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2024-03-22</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Arun Venugopal</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A new film about late New York Rep. Shirley Chisholm zeroes in on her 1972 Democratic presidential run, which was famously the first by a Black woman for any major political party.
-But at an advance screening of “Shirley” at BAM Rose Cinemas, a chief guardian of Chisholm's historical legacy argued that her greater significance is “not for being a first, but for someone who just sparked a fire,” and that she is as relevant to the present political moment as she was a half-century ago.
-“This film, I hope, allows you to be energized, to be motivated, to be inspired by Chisholm’s legacy,” said Zinga Fraser, director of the Shirley Chisholm Project of Brooklyn Women’s Activism at Brooklyn College. “She only wanted to be known as a catalyst for change.”
-"Shirley" follows in the footsteps of “Selma,” “Judas and the Black Messiah” and last year’s “Rustin” as the latest movie about a pivotal African American historical figure. But unlike those others, “Shirley,” which will begin streaming on Netflix on Friday after a brief theatrical run, is the relatively rare film to center a Black woman.
-"Shirley" was directed by John Ridley, who won the Academy Award for writing “12 Years a Slave.” It was also brought to the screen by two Black women: actress Regina King, who won an Academy Award for her role in “If Beale Street Could Talk” and plays Chisholm; and her sister Reina King, the movie’s producer, who plays Chisholm’s sister, Muriel. The King sisters have said for years that they wanted to bring Chisholm’s story to a wider audience.
-The movie doesn’t recount Chisholm’s childhood, her years in Barbados or her political rise in Brooklyn. It instead focuses on the excitement and shortcomings of Chisholm’s presidential run.
-“I’m paving the road for other people looking like me to get elected,” she says in the film, which also captures the tensions that arise as Chisholm’s supporters struggle to raise funds and increase her visibility.
-“This isn’t a campaign,” said her campaign manager Stanley Townsend, who is played by Brian Stokes Mitchell. “It’s a joke! The only thing anybody’s gonna remember is that there were a bunch of Black folks who made fools of themselves.”
-The Democratic nomination would ultimately be secured by Sen. George McGovern, whom incumbent Republican Richard Nixon would later defeat in a landslide during the 1972 general election.
-Chisholm is portrayed as determined and at times, from the perspective of her aides, obstinate to the point of being infuriating. After Alabama Gov. George Wallace — a staunch segregationist — barely survives an assassination attempt, Chisholm rejects the advice of her aides and goes to his bedside.
-In the movie, Chisholm is all too conscious of her candidacy's symbolism.
-“The people of America are watching us,” she said.
-The film has garnered mixed reviews. The Hollywood Reporter called it a “solid political bio that only sometimes matches its subject’s passion.” In a review for the New York Times, Devika Girish wrote that, “King is magnetic onscreen, nailing Chisholm’s accent and her steely persona. But there is little for her to do other than trade quips with the other characters, in a drama that is too content with telling rather than showing.”
-The film leaves out much of Chisholm’s important backstory, which may be a familiar journey for New Yorkers of a certain age.
-Chisholm was born in 1924 as Shirley Anita St. Hill in Brooklyn, but writes in her 1970 memoir “Unbought and Unbossed” that she was taken to Barbados at an early age to live with her grandmother. She returned to Brooklyn when she was 10 and lived with her parents and siblings in an "unheated, four-room, cold-water railroad flat" in Brownsville, which was a mostly-Jewish neighborhood at the time.
-She graduated from Brooklyn College and got her master’s degree in early childhood education from Columbia University in 1951 before eventually joining the League of Women Voters and the NAACP. In 1964, she became the second African American in the New York State Legislature and in 1968 she won a seat in Congress.
-A New York Times article from 1970 refers to her as “the frail‐looking, 100 pound educator from Brooklyn's 12th Congressional District” who had “consistently spoken out against the things she believes wrong and staunchly supported the causes she believes to be in the best interest of her urban, mostly poor Black constituents.” That same year she helped raise funds for Joan Bird, a Black Panther who was charged with attempted murder and eventually acquitted.
-Chisholm’s early years in Barbados are merely hinted at in the onscreen portrayal by King. Regina King called mastering Chisholm's fluctuating dialect – which shifted from Bajan to Brooklyn to something more scholarly – “terrifying.”
-Chisholm died in 2005 but her supporters argue that her convictions stand true and that she remains a model for anyone looking to effect change today.
-Writing in 1970, Chisholm argued that, “Our representative democracy is not working, because the Congress that is supposed to represent the voters does not respond to their needs. I believe the chief reason for this is that it is ruled by a small group of old men.”
-Speaking on WNYC’s "Brian Lehrer Show" in February, Fraser said Chisholm’s 1972 run was significant because it excited people “who were not necessarily involved in politics, but got involved in politics because Chisholm redefined what presidential elections should look like and who had the capability and should be able to run.”
-“She's saying, ‘This is not the domain of just white men,’” said Fraser. “‘We need to create a way in which we see ourselves at the highest levels in this country.’”
-</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>13</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/344083/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Indicted NJ Sen. Menendez 'hopeful' to run for reelection — but not with Democratic nod</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2024-03-21</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Louis C. Hochman</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sen. Robert Menendez — fighting corruption indictments for the second time in his political career — said he’s “hopeful” about running for a fourth term. But not with the Democratic nomination behind him.
-In a nine-minute video posted to YouTube Thursday, Menendez said he’s aiming for a summer exoneration that would “allow me to pursue my candidacy as an independent Democrat in the general election.”
-Menendez would have needed to submit petitions by Monday to run in the Democratic primary, where Rep. Andy Kim and Tammy Murphy are frontrunner candidates. He didn’t participate in any of the conventions that Democratic political machines use to decide who’ll get preferred placement on primary ballots — a tool party organizations and political bosses have used for a century to tip the scales in favor of their endorsed candidates.
-Campaigning after the Democratic primary, he said in the video, “would allow me the time to not only remind New Jerseyans of how I've succeeded in being your champion, but how we will secure our financial futures, meet the challenges of raising a family, owning a home, provide for a college education, and secure a more peaceful world for all of us to live in.”
-Menendez lost any practical chance of getting party endorsements or winning the Democratic nomination when the state’s most powerful political leaders — including Gov. Phil Murphy — called for him to step down days after his indictment in September.
-Menendez has maintained his innocence since his September indictment. But until now, he refused to say whether he’d seek reelection, even as Tammy Murphy and Kim far surpassed him in polling and fundraising, becoming clear frontrunners in a race to replace him.
-Earlier this month, Joseph Uribe — one of three businessmen accused of bribing Menendez and his wife with lavish gifts — pleaded guilty to federal charges and agreed to cooperate with the investigation against the senator.
-Prosecutors alleged in Menendez’s September indictment and later superseding indictments that he tried to interfere in criminal proceedings and did favors for the government of Egypt in exchange for gifts including gold bars and a Mercedes Benz. They later said he’d made public shows of support for Qatar to help one of the businessmen secure a deal with an investment fund where a member of the Qatari royal family was a principal.
-This month, prosecutors additionally charged Menendez and his wife with obstruction, saying they lied to their former lawyers about the gifts — describing them as loans — and caused those lawyers to repeat the same falsehoods to prosecutors.
-His trial is set to start in early May.
-“I know many of you are hurt and disappointed in me with the accusations I'm facing,” Menendez said in the video. “Believe me, I am disappointed at the false accusations as well.”
-Menendez, New Jersey’s senior senator, has long been a dominant figure in New Jersey politics — particularly Hudson County, where he began his political career on the Union City school board and as the city’s mayor before being elected to the state Legislature. He became a U.S. senator in 2006, first appointed to the role by then-Gov. Jon Corzine and later winning elections with strong party support.
-The leaders of Hudson County’s political organization lagged behind their peers in other county machines, when calls for Menendez to resign began pouring in the day of his indictment. But in November, the Hudson County Democratic Organization gave Murphy its endorsement.
-A poll by Monmouth University earlier this month found just 16% of respondents approved of the job Menendez is doing, and nearly three in four wanted him to step down.
-Menendez had just 9% support in a Fairleigh Dickinson University poll last month. .
-Menendez raised just $16,000, and refunded nearly the same amount, in the last quarter of 2023, NJ Monitor reported last month. In the same period, Murphy raised more than $3.2 million and Kim raised $1.8 million.
-Menendez's campaign committee and a separate defense fund also spent more than $2.6 million on legal fees in 2023, mostly related to the indictment, according to NJ Spotlight. Only his defense fund received significant donations after the indictment, and most of those contributions came from out-of-state donors, the report said.
-Menendez’s political career survived a previous bribery indictment. He was charged in 2015 with trading political favors for donations and other perks, but the trial ended in a hung jury.
-</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>17</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/344089/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Too late to change ballots NJ's political bosses use to sway elections? Judge pushes back.</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2024-03-19</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Nancy Solomon</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A federal judge questioned the claim that New Jersey’s county clerks don’t have time to reprint ballots before this year’s June primary elections — as he considers a case that could rob the state’s political machines of a tool that researchers say can decide an election before a single voter goes to the ballot box.
-But Judge Zahid N. Quraishi gave no timetable to rule on arguments he heard Monday from Rep. Andy Kim — who says the so-called “county line” ballot system used by 19 of New Jersey’s 21 counties violates his right to compete in a fair election. Kim testified that he is treated as an “underdog” compared to First Lady Tammy Murphy in the race for U.S. Senate, even as he enjoys a sizable lead in polls. Kim is seeking an injunction to get the unusual ballot system changed before the election is held.
-The “county line” has become the central issue in the Democratic primary for Senate. The little-understood quirk of New Jersey politics helps Democratic and Republican political organizations tip primary elections by awarding their endorsed candidates preferential placement on ballots — sometimes only on the say-so of those party organizations’ leaders. Research by academics from Princeton, Rutgers and Oxford says the line protects entrenched interests, giving endorsed candidates an advantage that outsiders rarely overcome.
-If the court were to find the county line unconstitutional, it would undo a system that has given the political machines tremendous power to influence which candidates ultimately win elected office as well — especially in areas that favor one party heavily, so there’s little competition after primaries. The same system once helped insulate incumbent Sen. Robert Menendez from political fallout after a 2015 corruption indictment, and turned against him amid another one in 2023. New Jersey hasn’t sent a Republican to the Senate in a half-century.
-That power structure is a huge advantage for Murphy — whose husband both heads New Jersey’s executive branch and effectively leads the state Democratic Party. In the first week after she declared her candidacy. Murphy was endorsed by the most powerful party leaders in the state.
-Quraishi listened to witness testimony in the case in a hearing that lasted more than nine hours. There were more than 20 lawyers representing the county clerks and three representing Kim, and the judge repeatedly rushed lawyers on both sides.
-Kim testified that when he first contemplated running for office for his first Congressional election in 2018, he quickly came to understand the power of the county line.
-“Literally the first question I was asked by anyone was whether I could get the county line,” Kim said on the stand. “In my first campaign, I wasn't taken seriously until I could show I had the county line. … It had a significant impact as to whether I’d be seen as viable by Democratic institutions.”
-The “line” places candidates endorsed by a county political organization into a single column or row — instead of putting all candidates for a given office in a list together, such as on the office-block ballots used in other states. Researchers say that gives candidates who share the line legitimacy before voters — particularly when a well-known political leader like President Joe Biden is in the first position.
-Kim testified he believes his ability to win his Senate campaign has been hurt by the county line. Kim has won placement on the line in most areas of New Jersey where party delegates cast secret ballots at conventions. But in most of the counties with the highest numbers of registered Democrats, county chairs who back Murphy awarded the line themselves.
-On Sunday, state Attorney General Matthew Platkin submitted a letter to the judge saying he would not oppose Kim’s request for an injunction, nor a related lawsuit seeking an end to the county line. Platkin’s five-page letter laid out his legal argument that the ballot system is unconstitutional. It earned a quick rebuke from Gov. Phil Murphy’s office — which says attorneys general typically defend state statutes, despite their own opinions.
-But before the hearing even got underway, Quraishi quickly signaled that he was not giving the letter from New Jersey’s top law enforcement official much weight.
-“It’s my call and not Mr. Platkin’s, and he’s well aware of that,” Quraishi said. “I have not decided whether I will consider that letter or the opinion of the AG.”
-Kim’s lawsuit names as defendants the county clerks from the 19 counties where the county line system is used. They say there is not enough time before the June primary to change the style of ballot.
-Monmouth County Clerk Christine Hanlon testified that changing to an office-block ballot would cause problems for her election operation.
-“I don’t know whether that can fit on the ballots we have today,” Hanlon testified. “There’s a limit to the number of grids on this system. You’d have to factor in how many of these office-blocks you could fit on the ballot and what order.”
-Hanlon said multi-page ballots would require a reprogramming of her scanners.
-She also testified that state statute requires the ballots to allow candidates to choose to associate with other candidates on the ballot by having their names listed in slates.
-“The statute requires columns and rows,” Hanlon said. “The bracketing statute provides that various candidates can opt to appear in the same column or row of the ballot.”
-Lawyers for the defendants called to the witness stand the owner of a printing company who prints the ballots for 11 county clerks. The printer, David Passante, said changing the ballot this close to the primary would cause chaos.
-But the judge challenged Passante.
-“If I order a change, you said it would be chaos. But what if one of the county clerks decides they want to do it differently. We prefer this kind of ballot in this county — do you tell them you can’t take their business?” Quraishi asked.
-“No,” Passante answered.
-Lawyers for Kim presented an election systems expert, Ryan Macias, who has 18 years experience in election systems, technology and administration. He testified that the software the county clerks use could easily spit out the office-block layout that Kim is requesting.
-To make their case that the county line gives an unfair advantage, Kim’s attorney’s entered a report by Rutgers Professor Julia Sass Rubin, who has published several studies on the county line, into the court record. Her research has found that congressional candidates who ran on the county line won on average by 35 points across dozens of races.
-The defense cross-examined Sass Rubin, asking her whether she could specify whether the races she analyzed could have been affected by name recognition of the candidate, or the amount of money spent on the race.
-“Potentially,” Sass Rubin said. “But you’re seeing the same pattern being on the county line and having the same results across 45 races.”
-The defense attorneys and clerks declined to comment on their way out of the courthouse. But Kim’s attorneys appeared to be in a much better mood.
-“We think it went well under the circumstances,” Yael Bromberg, one of Kim’s attorneys, said. “We only had a day to present evidence … and there were only three of us and a bevy of barristers, probably 50 attorneys on the other side."
-This story has been updated to correct David Passante's name.
-</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>24</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/343987/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Kim wins another NJ Dem convention for Senate, but numbers still good for Murphy</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2024-03-12</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Nancy Solomon</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Rep. Andy Kim won his seventh Democratic Party county convention on Monday, continuing his dominance over first lady Tammy Murphy at conventions — especially those where delegates are free to vote by secret ballot — as they both seek to replace Sen. Bob Menendez.
-But despite his popularity with rank-and-file Democrats, Kim still faces an uphill battle in the fight for endorsements that dictate how primary ballots are designed — and which candidate gets preferential placement. The counties he’s won so far are home to less than a fifth of New Jersey’s 2.5 million registered Democrats — and Murphy’s lined up endorsements in several large counties without a single delegate vote.
-Kim received 236 votes to Murphy’s 108, giving him Mercer’s sole endorsement. Mercer County awards any candidate with more than 40% of the vote a shared endorsement, but Murphy missed the mark with only 29% of the total votes cast.
-Patricia Campos Medina got 22 votes and Larry Hamm received 8 votes.
-Kim has won seven of the eight county conventions where delegates voted by secret ballot — taking victories in Monmouth, Hunterdon, Ocean, Sussex, Mercer, Burlington and Warren counties.
-The governor’s wife won her only secret ballot vote to date in Bergen County, where Kim says party leaders made it difficult for him to meet with members, though a county committee spokesperson denied that allegation. The county boss in Bergen, Paul Juliano, is a close ally of Gov. Phil Murphy with a lucrative state appointment who lobbied members extensively for the first lady.
-Murphy also took wins in Passaic, Union and Somerset counties. Passaic and Union counties only allow their leaderships to vote, and Somerset required its members to vote in full view of the party boss, who lobbied extensively for delegates to vote for Murphy.
-The candidates are battling for endorsements because in 19 of 21 counties in New Jersey, the party runs a slate of candidates in the primary on the “county line” — grouping them in a single row or column on primary ballots, and giving voters an impression of greater legitimacy. President Joe Biden will be listed at the top of the line this year. Tammy Murphy received personal endorsements from the party chairs in eight counties within a week of announcing she would run for the Senate.
-Kim and Murphy are running for the seat held by Menendez, who was indicted in September on charges of corruption, bribery and unregistered lobbying for a foreign government. Menendez, hasn’t said if he’ll pursue re-election but has yet to participate in any county party convention to date.
-Kim has made an issue of corruption and the county line, and has filed a lawsuit to stop the preferential placement on the ballot.
-“I am here, standing before you, not just as a candidate for Senate, not just as a three-term member of the House of Representatives, but as the father of a 6-year-old individual, terrified about what kind of America they're going to grow up in,” Kim told the Mercer County delegates. “Now is such a critical time for us to step up.”
-Murphy’s speech began with a reminder that she has often come to Mercer County, which is home to the state capitol.
-“Where Trenton goes, so goes the county, so goes our state,” Murphy told the delegates. “I have worshiped in the faith community. I've been to the Henry J. Austin Center [a community-based health center], visiting with moms. I've got a family festival here in Trenton. Importantly, I selected Trenton to be the home of the Infant and Maternal Innovation Health Center.”
-The Democratic political machines are strongest in the counties with the largest number of Democratic voters, largely because the chairs of the party committees are able to use their large number of voters as bargaining chips. They can use the county line on their ballots, and their large organizations of volunteers, to turn out votes.
-Despite Kim’s convincing wins in most conventions held so far, and his lead in a February poll, he still trails behind Murphy in the endorsement game by several important measures. The counties where Kim has so far received party endorsements represent 19% of registered Democrats in the state, while Murphy has already racked up endorsements in counties with 26% of Democrats.
-And that number does not include the counties where votes are not held at all, and Murphy has received the endorsements of the local county party boss. Those counties — Essex, Middlesex, Hudson and Camden — are home to 38% of the registered Democrats in the state but delegates aren't allowed to weigh in.
-In Mercer, not only were members allowed to vote by secret ballot, but there was no endorsement made by the Mercer County Democratic Committee chairwoman.
-“Mercer County has the best Democratic committee in New Jersey,” Janice Mironov, the committee chair, told the delegates.
-Next, the report on the rules for the meeting were explained and using Robert's Rules of Order, the membership voted to accept the rules.
-It was a change from the scenes that played out at some other county conventions.
-Party leaders in Hunterdon County tried to change the rules at the last minute to let anyone with at least 30% of the vote share the county line. That caused an uproar from the floor and a fight over whether the membership could challenge the party boss, ultimately defeating the rule change. Kim won that vote with 62% to Murphy’s 30%.
-Party members in Somerset County tried to get a vote from the floor on whether they could vote by secret ballot, and the party boss batted the rebels away, requiring members to vote by raising green cards.
-In Bergen, alternate and bonus delegates were allowed to vote.
-Cape May County Democrats also held their convention on Monday evening, but the leadership decided not to offer an endorsement. That usually happens when chairs of the county committees think their preferred candidates will lose the vote, according to Micah Rasmussen, director of the Rebovich Institute for New Jersey Politics.
-“[Murphy] spent the weekend in Cape May, so was clearly making a play there. If she had the votes, they’d have endorsed,” Rasmussen said. “This was a twin disappointment for Tammy Murphy. Her side clearly thought they had a shot in Mercer and they mobilized to hit that 40% mark, and did not reach it.”
-</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>17</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/343847/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>NY Republicans have an early voting problem. Could that spell trouble in 2024?</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2024-03-12</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Brigid Bergin</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">More than twice as many Democrats as Republicans voted early by mail in the race to represent the 3rd Congressional District in the U.S. House, a Gothamist analysis of the voter data for the special election found. And about a third more Democrats than Republicans opted for in-person early voting ahead of Election Day.
-The high early voting turnout was a key factor in Democrat Tom Suozzi’s victory in the 3rd Congressional District last month. Suozzi, who previously served in Congress, defeated Republican nominee Mazi Pilip by 8 points, making the turnout ahead of that snowy Election Day a critical buffer that helped secure his victory.
-New York state has seven competitive congressional races that could ultimately decide which party controls the U.S. House of Representatives, and New York Republicans are acknowledging that they have an early voting problem that needs to be fixed ahead of November’s elections.
-“We had President Trump basically in 2020 telling us not to do early voting, certainly downplaying it, and I think too many Republicans are still caught on that,” said Peter King, a Republican who represented parts of Long Island in Congress for three decades.
-King, who stepped down from his seat in 2021, said he never experienced a race where early voting and voting by mail played as crucial a role in the election as what he observed in the “Mazi Suozzi race.”
-In-person early voting took effect in New York in 2019, and gives voters nine days to vote before Election Day. The special election in the 3rd Congressional District was the first congressional election to also use the state’s new early vote-by-mail law, which meant nearly 1,000 votes had been cast a full month before the election.
-King said he personally isn't a fan of early voting, and likened it to picking the most valuable player in June — long before the baseball season ends. But he also stressed that “you got to play the game by the rules that are there, and the rules are now that early voting is becoming more and more important of a factor.”
-“We just have to up our game,” he added.
-Rep. Michael Lawler, whose Hudson Valley district is on the list of potential swing House seats in New York, said his campaign was taking a very deliberate approach to all aspects of voter engagement, including early voting.
-“We need to embrace it and make sure we are banking our vote,” Lawler told Gothamist.
-He said his campaign already has a track record of outperforming other Republicans in early voting.
-In this election, he said the campaign will use a host of tools including text messaging, robocalls, emails and digital ads to reach “low propensity voters.”
-“The objective is to get them to go vote,” said Lawler. “The reality is if the other side is going to utilize early voting and absentees to bank your vote, you can’t walk into Election Day with such a huge gap.”
-Nationally, Republicans have been reckoning with how to make up their early voting gap since last summer when the Republican National Committee launched an initiative called “Bank Your Vote,” which encouraged Republican voters to vote early in upcoming elections.
-The program was backed by former RNC Chair Ronna McDaniel, who resigned from her post on Friday. It’s unclear how much the RNC plans to push the “Bank Your Vote” initiative under its new leader, Michael Whatley, the head of the North Carolina Republican Party and a close ally of the party’s presumptive presidential nominee Donald Trump.
-A spokesperson for the RNC did not respond to repeated requests for comment.
-Savannah Viar, a spokesperson for the National Republican Congressional Committee did not comment directly on the Bank Your Vote initiative or early voting.
-“The NRCC is excited to continue working together with the RNC to win in November,” Viar said.
-The 3rd Congressional District, which stretches from eastern Queens through the northern part of Long Island, was an early bellwether for early voting and the outsize influence that casting a ballot ahead of Election Day may have.
-State voter enrollment data shows that the district has more active registered Democrats than Republicans, but even then, Democrats turned out in greater numbers than expected.
-Democrats make up just under 40% of active registered voters but accounted for 44% of in-person early votes and a whopping 55% of early votes by mail, according to Gothamist’s analysis.
-On top of the early voting deficit Republicans faced ahead of the Feb. 13 special election, voters also confronted one of the few major snowstorms of this winter.
-The weather was so bad that a spokesperson for the Congressional Leadership Fund, a super PAC that aims to elect Republicans to the U.S. House, told Gothamist at the time that they hired extra snowplows to help clear streets in Republican portions of the district that day.
-After the polls closed, Nassau County GOP Chair Joseph Cairo told Gothamist that he believed the snow depressed turnout on Election Day, though not enough to decide the race.
-His spokesperson did not respond to requests for comment about how the party has analyzed other factors that led to its loss and how much it plans to emphasize early voting going forward.
-The state GOP launched its own version of the “Bank Your Vote” campaign last September with GOP Chair Rep. Elise Stefanik. The program targets voters based on GOP data who are likely to vote before Election Day and asks them to apply for a mail ballot or pledge to vote early.
-State GOP spokesperson David Laska told Gothamist that the state party still plans to build on the momentum of the RNC’s Bank Your Vote’ campaign, “because when Republicans vote early, we win.”
-“We will defend our majority-making congressional delegation in 2024 with President Trump and his endorsed candidate Mike Sapraicone at the top of the ticket,” Laska added, in reference to the Republican Party’s U.S. Senate candidate running against Sen. Kirsten Gillibrand, a Democrat who is up for re-election this year.
-Jon Campbell and Michelle Bocanegra contributed reporting.
-</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>29</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/343832/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>NY Gov. Hochul leans hard into role as Biden surrogate</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2024-03-11</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Jon Campbell</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Plenty of New Yorkers have their doubts about President Joe Biden, polls show. But Gov. Kathy Hochul isn’t among them.
-The Democratic governor attended Biden’s State of the Union address on Thursday in Washington, D.C., and lauded his “vision for our future.” Days earlier, on Super Tuesday, she touted his electoral prospects on CNN. And for weeks, she’s been jabbing at former president Donald Trump and House Republicans for tanking a bipartisan deal on border security — echoing a key Biden talking point.
-It's something of a new role for Hochul, who is now leaning heavily into national politics and her position as the de facto head of New York’s Democratic Party. She appears intent to prove herself as a loyal Biden supporter and reliable espouser of Democratic leaders’ views, particularly on immigration and abortion.
-And it could be a sign of things to come: Hochul is pledging to be an active voice in the 2024 presidential and House elections, even though she’s not on the ballot herself.
-“When the story gets out of [Biden’s] record of accomplishment, people are going to say ‘why did we even entertain going with Donald Trump?’” Hochul said during her CNN appearance. “Let's stick with the competent leadership, the trusted leadership, and that'll get us through the next four years.”
-A Siena College poll last month showed Biden’s approval rating under water in New York, with 52% of voters disapproving of his job performance and 45% approving.
-But the Democratic president isn’t in any serious danger of losing the deep-blue state, which has voted for the Democratic presidential candidate in every election since Ronald Reagan won in a national landslide in 1984. The Siena poll showed Biden defeating Trump by 12 points in a head-to-head matchup in New York.
-To be sure, Hochul hasn’t always agreed with Biden. Her and New York City Mayor Eric Adams’ push for additional federal funds to help with tens of thousands of migrants seeking shelter in the city has yet to be granted.
-But unlike Adams, Hochul has stayed largely positive when speaking publicly about the Biden administration. It has kept the governor in the rotation of Biden surrogates on cable news, especially when House Republicans declined to support a Senate-negotiated measure tightening restrictions on seeking asylum in United States.
-Basil Smikle, a Columbia University lecturer who previously served as executive director of the New York State Democratic Committee, said Hochul has a significant role to play as the party's leader in New York this year.
-“She's going to be representing the state of New York in this election in a way that Democratic governors haven't had to in a long time," he said. "The state generally doesn't feature very heavily in presidential politics, but it will this year because Democratic control of the House goes through New York."
-According to some political observers, Hochul’s performance as a gubernatorial candidate in 2022 contributed to Democrats ceding control of the House in the first place.
-She defeated Republican Lee Zeldin by six points that year, a less-than-robust showing that trickled down the ballot and affected other races in the state. This was particularly true in the Hudson Valley and Long Island, where Hochul’s performance lagged behind that of Biden two years earlier — helping a handful of Republicans flip congressional seats.
-Since then, Hochul has taken a more aggressive approach politically.
-She’s repeatedly called out New York’s 10 House Republicans in recent weeks, attempting to blame them for Washington’s inaction on border security.
-She’s also adopted a tough-on-crime stance, most notably by sending the National Guard into the New York City subway system to assist NYPD officers with checking riders' bags for weapons. Hochul acknowledged the move was at least partly designed to undermine a Republican talking point and show “Democrats fight crime as well.”
-Republican Rep. Mike Lawler, one of Democrats’ top targets in this year's House elections who faces a challenge from former Democratic Rep. Mondaire Jones in the Hudson Valley, said he wasn't concerned about Hochul potentially taking an active role in his race. He said he actually would welcome it.
-“The American people aren't stupid and New Yorkers aren't stupid,” Lawler said in an interview. “They realize who's in charge and they realize that [the migrant influx] is a result of the disastrous policies that Joe Biden and Kathy Hochul have enacted.”
-In some cases, House Republicans have tried to bait Hochul into taking them on, perhaps buoyed by her underwhelming performance in their districts in 2022. That includes Rep. Marc Molinaro, who represents a swing district in the Hudson Valley and Southern Tier that stretches up to the Albany area.
-After Bronx Rep. Adriano Espaillat announced Hochul would be his guest for Biden’s State of the Union speech, Molinaro issued a press release calling on the governor to meet with him in Washington and providing his office number so that the governor's staffers could easily get in touch with his own.
-“We clearly have different approaches, but the rhetoric and verbal sparring isn’t helping those in New York feeling the impact of this crisis,” he said in a statement.
-Hochul has dismissed such invitations from New York Republicans as political stunts. Her campaign spokesperson, Jen Goodman, said the governor will continue to hit the campaign trail hard this year.
-“From New York’s vulnerable House Republicans to the threat of a Trump presidency, Governor Hochul will continue to make the case to voters just how much is at stake in 2024,” Goodman said.
-</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>24</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/343815/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Expelled from Congress, George Santos will run again in neighboring NY district</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2024-03-08</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Brittany Kriegstein</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">He fabricated much of his own biography, was expelled from the House of Representatives and is facing federal criminal charges.
-But George Santos decided it’s a good time to run for Congress – again.
-The Republican made the announcement on X during President Joe Biden’s State of the Union address.
-“After a lot of prayer and conversation with my friends and family, I have made a very important decision that will shake things up,” Santos wrote, after calling Biden a “weak, frail president” who had delivered “spin and lies to the American people.”
-Santos said he will be challenging fellow Republican Nick LaLota for control of New York’s Congressional District 1, which includes the Long Island towns of Huntington, Smithtown, Riverhead, Southold, Southampton, East Hampton, and Shelter Island.
-It’s right next door to the district from which he was formally expelled by his fellow members of Congress in a 311-114, bipartisan vote after a damning report from a House ethics subcommittee found “substantial evidence” of misconduct and illegal activity on top of the federal indictment. Santos’ expulsion led to a special election that resulted in Republicans losing the seat to veteran Democrat Tom Suozzi.
-But Santos glossed over those details in his announcement, insisting he’d left office “arbitrarily” and taking aim at LaLota.
-“He is a willing [sic] to risk the future of our majority and the future of this country for his own political gain,” Santos wrote. “I look forward to debating him on the issues and on his weak record as a Republican.”
-LaLota, a vocal proponent of Santos’ expulsion from Congress last year, said in a statement that he welcomed the challenge.
-“To raise the standard in Congress, and to hold a pathological liar who stole an election accountable, I led the charge to expel George Santos," LaLota said. "If finishing the job requires beating him in a primary, count me in.”
-As of Friday morning, Santos’ website had not yet been updated to reflect his District 1 bid – instead asking prospective donors to “help us take back New York’s third district for the people.”
-</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>5</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>https://cms.prod.nypr.digital/images/343797/fill-700x467|format-webp|webpquality-70/</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>